<commit_message>
[sil_euro_latin] support n dieresis
</commit_message>
<xml_diff>
--- a/release/sil/sil_euro_latin/assets/EuroLatinChart.xlsx
+++ b/release/sil/sil_euro_latin/assets/EuroLatinChart.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0WSTech\working\keyboards\release\sil\sil_euro_latin\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\NRSI\keyboards_testing\release\x\sil_euro_latin\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="15570" windowHeight="11310"/>
+    <workbookView xWindow="360" yWindow="108" windowWidth="15576" windowHeight="11316"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="717">
   <si>
     <t>a</t>
   </si>
@@ -2166,12 +2166,18 @@
   </si>
   <si>
     <t>Ḉ</t>
+  </si>
+  <si>
+    <t>N̈</t>
+  </si>
+  <si>
+    <t>n̈</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -2968,21 +2974,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BC59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="AC40" sqref="AC40"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="3.140625" style="4" customWidth="1"/>
-    <col min="3" max="30" width="3.140625" style="2" customWidth="1"/>
-    <col min="31" max="31" width="9.140625" style="2"/>
-    <col min="32" max="58" width="5.28515625" style="2" customWidth="1"/>
-    <col min="59" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.109375" style="2"/>
+    <col min="2" max="2" width="3.109375" style="4" customWidth="1"/>
+    <col min="3" max="30" width="3.109375" style="2" customWidth="1"/>
+    <col min="31" max="31" width="9.109375" style="2"/>
+    <col min="32" max="58" width="5.33203125" style="2" customWidth="1"/>
+    <col min="59" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:55" ht="16.5" thickBot="1">
+    <row r="2" spans="2:55" ht="15.6" thickBot="1">
       <c r="C2" s="3" t="s">
         <v>50</v>
       </c>
@@ -2990,7 +2996,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="3" spans="2:55" ht="16.5" thickBot="1">
+    <row r="3" spans="2:55" ht="15.6" thickBot="1">
       <c r="B3" s="11" t="s">
         <v>28</v>
       </c>
@@ -3038,7 +3044,7 @@
       <c r="AB3" s="13"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="2:55" ht="21.75">
+    <row r="4" spans="2:55" ht="23.4">
       <c r="B4" s="5" t="s">
         <v>27</v>
       </c>
@@ -3151,7 +3157,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="5" spans="2:55" ht="16.5" thickBot="1">
+    <row r="5" spans="2:55" ht="15.6" thickBot="1">
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -3322,7 +3328,7 @@
       <c r="AB6" s="7"/>
       <c r="AC6" s="9"/>
     </row>
-    <row r="7" spans="2:55" ht="16.5" thickBot="1">
+    <row r="7" spans="2:55" ht="15.6" thickBot="1">
       <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
@@ -3383,7 +3389,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="8" spans="2:55" ht="21.75">
+    <row r="8" spans="2:55" ht="23.4">
       <c r="B8" s="5" t="s">
         <v>31</v>
       </c>
@@ -3497,7 +3503,7 @@
       <c r="AW8" s="1"/>
       <c r="AX8" s="1"/>
     </row>
-    <row r="9" spans="2:55" ht="16.5" thickBot="1">
+    <row r="9" spans="2:55" ht="15.6" thickBot="1">
       <c r="B9" s="5" t="s">
         <v>389</v>
       </c>
@@ -3583,7 +3589,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="10" spans="2:55" ht="16.5" thickBot="1">
+    <row r="10" spans="2:55" ht="15.6" thickBot="1">
       <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
@@ -3629,7 +3635,7 @@
       <c r="AB10" s="7"/>
       <c r="AC10" s="9"/>
     </row>
-    <row r="11" spans="2:55" ht="21.75">
+    <row r="11" spans="2:55" ht="23.4">
       <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
@@ -3726,7 +3732,7 @@
       <c r="BB11" s="1"/>
       <c r="BC11" s="1"/>
     </row>
-    <row r="12" spans="2:55" ht="16.5" thickBot="1">
+    <row r="12" spans="2:55" ht="15.6" thickBot="1">
       <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
@@ -3898,7 +3904,9 @@
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
-      <c r="P14" s="7"/>
+      <c r="P14" s="8" t="s">
+        <v>716</v>
+      </c>
       <c r="Q14" s="8" t="s">
         <v>261</v>
       </c>
@@ -3976,7 +3984,7 @@
       <c r="AB15" s="7"/>
       <c r="AC15" s="9"/>
     </row>
-    <row r="16" spans="2:55" ht="16.5" thickBot="1">
+    <row r="16" spans="2:55" ht="15.6" thickBot="1">
       <c r="B16" s="5" t="s">
         <v>37</v>
       </c>
@@ -4055,7 +4063,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="17" spans="2:54" ht="21.75">
+    <row r="17" spans="2:54" ht="23.4">
       <c r="B17" s="5" t="s">
         <v>420</v>
       </c>
@@ -4148,7 +4156,7 @@
       <c r="AY17" s="1"/>
       <c r="AZ17" s="1"/>
     </row>
-    <row r="18" spans="2:54" ht="16.5" thickBot="1">
+    <row r="18" spans="2:54" ht="15.6" thickBot="1">
       <c r="B18" s="5" t="s">
         <v>38</v>
       </c>
@@ -4232,7 +4240,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="19" spans="2:54" ht="16.5" thickBot="1">
+    <row r="19" spans="2:54" ht="15.6" thickBot="1">
       <c r="B19" s="5" t="s">
         <v>39</v>
       </c>
@@ -4288,7 +4296,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="20" spans="2:54" ht="19.149999999999999" customHeight="1">
+    <row r="20" spans="2:54" ht="19.2" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>40</v>
       </c>
@@ -4371,7 +4379,7 @@
       <c r="AX20" s="1"/>
       <c r="AY20" s="1"/>
     </row>
-    <row r="21" spans="2:54" ht="16.5" thickBot="1">
+    <row r="21" spans="2:54" ht="15.6" thickBot="1">
       <c r="B21" s="20"/>
       <c r="C21" s="21" t="s">
         <v>0</v>
@@ -4485,7 +4493,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="22" spans="2:54" ht="16.5" thickBot="1">
+    <row r="22" spans="2:54" ht="15.6" thickBot="1">
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
@@ -4515,7 +4523,7 @@
       <c r="AB22" s="23"/>
       <c r="AC22" s="23"/>
     </row>
-    <row r="23" spans="2:54" ht="22.5" thickBot="1">
+    <row r="23" spans="2:54" ht="24" thickBot="1">
       <c r="C23" s="3" t="s">
         <v>51</v>
       </c>
@@ -4572,7 +4580,7 @@
       <c r="BA23" s="1"/>
       <c r="BB23" s="1"/>
     </row>
-    <row r="24" spans="2:54" ht="16.5" thickBot="1">
+    <row r="24" spans="2:54" ht="15.6" thickBot="1">
       <c r="B24" s="11" t="s">
         <v>28</v>
       </c>
@@ -5214,7 +5222,9 @@
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="7"/>
+      <c r="P35" s="8" t="s">
+        <v>715</v>
+      </c>
       <c r="Q35" s="8" t="s">
         <v>325</v>
       </c>
@@ -5583,7 +5593,7 @@
       <c r="AB41" s="17"/>
       <c r="AC41" s="19"/>
     </row>
-    <row r="42" spans="2:32" ht="16.5" thickBot="1">
+    <row r="42" spans="2:32" ht="15.6" thickBot="1">
       <c r="B42" s="20"/>
       <c r="C42" s="21" t="s">
         <v>52</v>
@@ -5703,7 +5713,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="2:32" s="1" customFormat="1" ht="15" thickBot="1">
+    <row r="45" spans="2:32" s="1" customFormat="1" ht="14.4" thickBot="1">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -5795,7 +5805,7 @@
       </c>
       <c r="AF46" s="4"/>
     </row>
-    <row r="47" spans="2:32" ht="15" thickBot="1">
+    <row r="47" spans="2:32" ht="14.4" thickBot="1">
       <c r="B47" s="24" t="s">
         <v>632</v>
       </c>
@@ -5867,7 +5877,7 @@
       <c r="B48" s="2"/>
       <c r="AF48" s="4"/>
     </row>
-    <row r="49" spans="2:23" s="1" customFormat="1" ht="16.5" thickBot="1">
+    <row r="49" spans="2:23" s="1" customFormat="1" ht="15.6" thickBot="1">
       <c r="B49" s="3" t="s">
         <v>657</v>
       </c>
@@ -5893,7 +5903,7 @@
       <c r="V49" s="2"/>
       <c r="W49" s="2"/>
     </row>
-    <row r="50" spans="2:23" s="35" customFormat="1" ht="14.25">
+    <row r="50" spans="2:23" s="35" customFormat="1" ht="13.8">
       <c r="B50" s="30" t="s">
         <v>658</v>
       </c>
@@ -5953,7 +5963,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="51" spans="2:23" s="32" customFormat="1" ht="15" thickBot="1">
+    <row r="51" spans="2:23" s="32" customFormat="1" ht="14.4" thickBot="1">
       <c r="B51" s="33" t="s">
         <v>659</v>
       </c>
@@ -6013,15 +6023,15 @@
         <v>690</v>
       </c>
     </row>
-    <row r="52" spans="2:23" s="1" customFormat="1" ht="14.25"/>
-    <row r="53" spans="2:23" ht="14.25">
+    <row r="52" spans="2:23" s="1" customFormat="1" ht="13.8"/>
+    <row r="53" spans="2:23" ht="13.8">
       <c r="B53" s="2"/>
     </row>
-    <row r="55" spans="2:23" s="1" customFormat="1" ht="14.25"/>
-    <row r="56" spans="2:23" ht="14.25">
+    <row r="55" spans="2:23" s="1" customFormat="1" ht="13.8"/>
+    <row r="56" spans="2:23" ht="13.8">
       <c r="B56" s="2"/>
     </row>
-    <row r="59" spans="2:23" s="1" customFormat="1" ht="14.25">
+    <row r="59" spans="2:23" s="1" customFormat="1" ht="13.8">
       <c r="B59" s="2"/>
     </row>
   </sheetData>
@@ -6036,7 +6046,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6048,7 +6058,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Revert "update from master"
This reverts commit d1f9dacce7dd3cdd35c3e53df952f6c9cd7e7225.
</commit_message>
<xml_diff>
--- a/release/sil/sil_euro_latin/assets/EuroLatinChart.xlsx
+++ b/release/sil/sil_euro_latin/assets/EuroLatinChart.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\NRSI\keyboards_testing\release\x\sil_euro_latin\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0WSTech\working\keyboards\release\sil\sil_euro_latin\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="108" windowWidth="15576" windowHeight="11316"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="15570" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="715">
   <si>
     <t>a</t>
   </si>
@@ -2166,18 +2166,12 @@
   </si>
   <si>
     <t>Ḉ</t>
-  </si>
-  <si>
-    <t>N̈</t>
-  </si>
-  <si>
-    <t>n̈</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -2974,21 +2968,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:BC59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="AC40" sqref="AC40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="3.109375" style="4" customWidth="1"/>
-    <col min="3" max="30" width="3.109375" style="2" customWidth="1"/>
-    <col min="31" max="31" width="9.109375" style="2"/>
-    <col min="32" max="58" width="5.33203125" style="2" customWidth="1"/>
-    <col min="59" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="3.140625" style="4" customWidth="1"/>
+    <col min="3" max="30" width="3.140625" style="2" customWidth="1"/>
+    <col min="31" max="31" width="9.140625" style="2"/>
+    <col min="32" max="58" width="5.28515625" style="2" customWidth="1"/>
+    <col min="59" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:55" ht="15.6" thickBot="1">
+    <row r="2" spans="2:55" ht="16.5" thickBot="1">
       <c r="C2" s="3" t="s">
         <v>50</v>
       </c>
@@ -2996,7 +2990,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="3" spans="2:55" ht="15.6" thickBot="1">
+    <row r="3" spans="2:55" ht="16.5" thickBot="1">
       <c r="B3" s="11" t="s">
         <v>28</v>
       </c>
@@ -3044,7 +3038,7 @@
       <c r="AB3" s="13"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="2:55" ht="23.4">
+    <row r="4" spans="2:55" ht="21.75">
       <c r="B4" s="5" t="s">
         <v>27</v>
       </c>
@@ -3157,7 +3151,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="5" spans="2:55" ht="15.6" thickBot="1">
+    <row r="5" spans="2:55" ht="16.5" thickBot="1">
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -3328,7 +3322,7 @@
       <c r="AB6" s="7"/>
       <c r="AC6" s="9"/>
     </row>
-    <row r="7" spans="2:55" ht="15.6" thickBot="1">
+    <row r="7" spans="2:55" ht="16.5" thickBot="1">
       <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
@@ -3389,7 +3383,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="8" spans="2:55" ht="23.4">
+    <row r="8" spans="2:55" ht="21.75">
       <c r="B8" s="5" t="s">
         <v>31</v>
       </c>
@@ -3503,7 +3497,7 @@
       <c r="AW8" s="1"/>
       <c r="AX8" s="1"/>
     </row>
-    <row r="9" spans="2:55" ht="15.6" thickBot="1">
+    <row r="9" spans="2:55" ht="16.5" thickBot="1">
       <c r="B9" s="5" t="s">
         <v>389</v>
       </c>
@@ -3589,7 +3583,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="10" spans="2:55" ht="15.6" thickBot="1">
+    <row r="10" spans="2:55" ht="16.5" thickBot="1">
       <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
@@ -3635,7 +3629,7 @@
       <c r="AB10" s="7"/>
       <c r="AC10" s="9"/>
     </row>
-    <row r="11" spans="2:55" ht="23.4">
+    <row r="11" spans="2:55" ht="21.75">
       <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
@@ -3732,7 +3726,7 @@
       <c r="BB11" s="1"/>
       <c r="BC11" s="1"/>
     </row>
-    <row r="12" spans="2:55" ht="15.6" thickBot="1">
+    <row r="12" spans="2:55" ht="16.5" thickBot="1">
       <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
@@ -3904,9 +3898,7 @@
       <c r="M14" s="7"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
-      <c r="P14" s="8" t="s">
-        <v>716</v>
-      </c>
+      <c r="P14" s="7"/>
       <c r="Q14" s="8" t="s">
         <v>261</v>
       </c>
@@ -3984,7 +3976,7 @@
       <c r="AB15" s="7"/>
       <c r="AC15" s="9"/>
     </row>
-    <row r="16" spans="2:55" ht="15.6" thickBot="1">
+    <row r="16" spans="2:55" ht="16.5" thickBot="1">
       <c r="B16" s="5" t="s">
         <v>37</v>
       </c>
@@ -4063,7 +4055,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="17" spans="2:54" ht="23.4">
+    <row r="17" spans="2:54" ht="21.75">
       <c r="B17" s="5" t="s">
         <v>420</v>
       </c>
@@ -4156,7 +4148,7 @@
       <c r="AY17" s="1"/>
       <c r="AZ17" s="1"/>
     </row>
-    <row r="18" spans="2:54" ht="15.6" thickBot="1">
+    <row r="18" spans="2:54" ht="16.5" thickBot="1">
       <c r="B18" s="5" t="s">
         <v>38</v>
       </c>
@@ -4240,7 +4232,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="19" spans="2:54" ht="15.6" thickBot="1">
+    <row r="19" spans="2:54" ht="16.5" thickBot="1">
       <c r="B19" s="5" t="s">
         <v>39</v>
       </c>
@@ -4296,7 +4288,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="20" spans="2:54" ht="19.2" customHeight="1">
+    <row r="20" spans="2:54" ht="19.149999999999999" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>40</v>
       </c>
@@ -4379,7 +4371,7 @@
       <c r="AX20" s="1"/>
       <c r="AY20" s="1"/>
     </row>
-    <row r="21" spans="2:54" ht="15.6" thickBot="1">
+    <row r="21" spans="2:54" ht="16.5" thickBot="1">
       <c r="B21" s="20"/>
       <c r="C21" s="21" t="s">
         <v>0</v>
@@ -4493,7 +4485,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="22" spans="2:54" ht="15.6" thickBot="1">
+    <row r="22" spans="2:54" ht="16.5" thickBot="1">
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
@@ -4523,7 +4515,7 @@
       <c r="AB22" s="23"/>
       <c r="AC22" s="23"/>
     </row>
-    <row r="23" spans="2:54" ht="24" thickBot="1">
+    <row r="23" spans="2:54" ht="22.5" thickBot="1">
       <c r="C23" s="3" t="s">
         <v>51</v>
       </c>
@@ -4580,7 +4572,7 @@
       <c r="BA23" s="1"/>
       <c r="BB23" s="1"/>
     </row>
-    <row r="24" spans="2:54" ht="15.6" thickBot="1">
+    <row r="24" spans="2:54" ht="16.5" thickBot="1">
       <c r="B24" s="11" t="s">
         <v>28</v>
       </c>
@@ -5222,9 +5214,7 @@
       <c r="M35" s="7"/>
       <c r="N35" s="7"/>
       <c r="O35" s="7"/>
-      <c r="P35" s="8" t="s">
-        <v>715</v>
-      </c>
+      <c r="P35" s="7"/>
       <c r="Q35" s="8" t="s">
         <v>325</v>
       </c>
@@ -5593,7 +5583,7 @@
       <c r="AB41" s="17"/>
       <c r="AC41" s="19"/>
     </row>
-    <row r="42" spans="2:32" ht="15.6" thickBot="1">
+    <row r="42" spans="2:32" ht="16.5" thickBot="1">
       <c r="B42" s="20"/>
       <c r="C42" s="21" t="s">
         <v>52</v>
@@ -5713,7 +5703,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="2:32" s="1" customFormat="1" ht="14.4" thickBot="1">
+    <row r="45" spans="2:32" s="1" customFormat="1" ht="15" thickBot="1">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -5805,7 +5795,7 @@
       </c>
       <c r="AF46" s="4"/>
     </row>
-    <row r="47" spans="2:32" ht="14.4" thickBot="1">
+    <row r="47" spans="2:32" ht="15" thickBot="1">
       <c r="B47" s="24" t="s">
         <v>632</v>
       </c>
@@ -5877,7 +5867,7 @@
       <c r="B48" s="2"/>
       <c r="AF48" s="4"/>
     </row>
-    <row r="49" spans="2:23" s="1" customFormat="1" ht="15.6" thickBot="1">
+    <row r="49" spans="2:23" s="1" customFormat="1" ht="16.5" thickBot="1">
       <c r="B49" s="3" t="s">
         <v>657</v>
       </c>
@@ -5903,7 +5893,7 @@
       <c r="V49" s="2"/>
       <c r="W49" s="2"/>
     </row>
-    <row r="50" spans="2:23" s="35" customFormat="1" ht="13.8">
+    <row r="50" spans="2:23" s="35" customFormat="1" ht="14.25">
       <c r="B50" s="30" t="s">
         <v>658</v>
       </c>
@@ -5963,7 +5953,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="51" spans="2:23" s="32" customFormat="1" ht="14.4" thickBot="1">
+    <row r="51" spans="2:23" s="32" customFormat="1" ht="15" thickBot="1">
       <c r="B51" s="33" t="s">
         <v>659</v>
       </c>
@@ -6023,15 +6013,15 @@
         <v>690</v>
       </c>
     </row>
-    <row r="52" spans="2:23" s="1" customFormat="1" ht="13.8"/>
-    <row r="53" spans="2:23" ht="13.8">
+    <row r="52" spans="2:23" s="1" customFormat="1" ht="14.25"/>
+    <row r="53" spans="2:23" ht="14.25">
       <c r="B53" s="2"/>
     </row>
-    <row r="55" spans="2:23" s="1" customFormat="1" ht="13.8"/>
-    <row r="56" spans="2:23" ht="13.8">
+    <row r="55" spans="2:23" s="1" customFormat="1" ht="14.25"/>
+    <row r="56" spans="2:23" ht="14.25">
       <c r="B56" s="2"/>
     </row>
-    <row r="59" spans="2:23" s="1" customFormat="1" ht="13.8">
+    <row r="59" spans="2:23" s="1" customFormat="1" ht="14.25">
       <c r="B59" s="2"/>
     </row>
   </sheetData>
@@ -6046,7 +6036,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6058,7 +6048,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[sil_euro_latin] Add support for j-acute
</commit_message>
<xml_diff>
--- a/release/sil/sil_euro_latin/assets/EuroLatinChart.xlsx
+++ b/release/sil/sil_euro_latin/assets/EuroLatinChart.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents\NRSI\keyboards_testing\release\x\sil_euro_latin\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0WSTech\working\keyboards\release\todo\sil_euro_latin\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DA3E55-19F4-4869-ADF4-3CCB9ED1414B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="108" windowWidth="15576" windowHeight="11316"/>
+    <workbookView xWindow="360" yWindow="105" windowWidth="15570" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="719">
   <si>
     <t>a</t>
   </si>
@@ -2172,12 +2173,18 @@
   </si>
   <si>
     <t>n̈</t>
+  </si>
+  <si>
+    <t>j́</t>
+  </si>
+  <si>
+    <t>J́</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
       <sz val="11"/>
@@ -2761,6 +2768,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2796,6 +2820,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2971,24 +3012,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:BC59"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="2"/>
-    <col min="2" max="2" width="3.109375" style="4" customWidth="1"/>
-    <col min="3" max="30" width="3.109375" style="2" customWidth="1"/>
-    <col min="31" max="31" width="9.109375" style="2"/>
-    <col min="32" max="58" width="5.33203125" style="2" customWidth="1"/>
-    <col min="59" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="3.140625" style="4" customWidth="1"/>
+    <col min="3" max="30" width="3.140625" style="2" customWidth="1"/>
+    <col min="31" max="31" width="9.140625" style="2"/>
+    <col min="32" max="58" width="5.28515625" style="2" customWidth="1"/>
+    <col min="59" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:55" ht="15.6" thickBot="1">
+    <row r="2" spans="2:55" ht="16.5" thickBot="1">
       <c r="C2" s="3" t="s">
         <v>50</v>
       </c>
@@ -2996,7 +3037,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="3" spans="2:55" ht="15.6" thickBot="1">
+    <row r="3" spans="2:55" ht="16.5" thickBot="1">
       <c r="B3" s="11" t="s">
         <v>28</v>
       </c>
@@ -3044,7 +3085,7 @@
       <c r="AB3" s="13"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="2:55" ht="23.4">
+    <row r="4" spans="2:55" ht="21.75">
       <c r="B4" s="5" t="s">
         <v>27</v>
       </c>
@@ -3157,7 +3198,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="5" spans="2:55" ht="15.6" thickBot="1">
+    <row r="5" spans="2:55" ht="16.5" thickBot="1">
       <c r="B5" s="5" t="s">
         <v>26</v>
       </c>
@@ -3180,7 +3221,9 @@
       <c r="K5" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="L5" s="7"/>
+      <c r="L5" s="8" t="s">
+        <v>717</v>
+      </c>
       <c r="M5" s="8" t="s">
         <v>120</v>
       </c>
@@ -3328,7 +3371,7 @@
       <c r="AB6" s="7"/>
       <c r="AC6" s="9"/>
     </row>
-    <row r="7" spans="2:55" ht="15.6" thickBot="1">
+    <row r="7" spans="2:55" ht="16.5" thickBot="1">
       <c r="B7" s="5" t="s">
         <v>30</v>
       </c>
@@ -3389,7 +3432,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="8" spans="2:55" ht="23.4">
+    <row r="8" spans="2:55" ht="21.75">
       <c r="B8" s="5" t="s">
         <v>31</v>
       </c>
@@ -3503,7 +3546,7 @@
       <c r="AW8" s="1"/>
       <c r="AX8" s="1"/>
     </row>
-    <row r="9" spans="2:55" ht="15.6" thickBot="1">
+    <row r="9" spans="2:55" ht="16.5" thickBot="1">
       <c r="B9" s="5" t="s">
         <v>389</v>
       </c>
@@ -3589,7 +3632,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="10" spans="2:55" ht="15.6" thickBot="1">
+    <row r="10" spans="2:55" ht="16.5" thickBot="1">
       <c r="B10" s="5" t="s">
         <v>32</v>
       </c>
@@ -3635,7 +3678,7 @@
       <c r="AB10" s="7"/>
       <c r="AC10" s="9"/>
     </row>
-    <row r="11" spans="2:55" ht="23.4">
+    <row r="11" spans="2:55" ht="21.75">
       <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
@@ -3732,7 +3775,7 @@
       <c r="BB11" s="1"/>
       <c r="BC11" s="1"/>
     </row>
-    <row r="12" spans="2:55" ht="15.6" thickBot="1">
+    <row r="12" spans="2:55" ht="16.5" thickBot="1">
       <c r="B12" s="5" t="s">
         <v>34</v>
       </c>
@@ -3984,7 +4027,7 @@
       <c r="AB15" s="7"/>
       <c r="AC15" s="9"/>
     </row>
-    <row r="16" spans="2:55" ht="15.6" thickBot="1">
+    <row r="16" spans="2:55" ht="16.5" thickBot="1">
       <c r="B16" s="5" t="s">
         <v>37</v>
       </c>
@@ -4063,7 +4106,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="17" spans="2:54" ht="23.4">
+    <row r="17" spans="2:54" ht="21.75">
       <c r="B17" s="5" t="s">
         <v>420</v>
       </c>
@@ -4156,7 +4199,7 @@
       <c r="AY17" s="1"/>
       <c r="AZ17" s="1"/>
     </row>
-    <row r="18" spans="2:54" ht="15.6" thickBot="1">
+    <row r="18" spans="2:54" ht="16.5" thickBot="1">
       <c r="B18" s="5" t="s">
         <v>38</v>
       </c>
@@ -4240,7 +4283,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="19" spans="2:54" ht="15.6" thickBot="1">
+    <row r="19" spans="2:54" ht="16.5" thickBot="1">
       <c r="B19" s="5" t="s">
         <v>39</v>
       </c>
@@ -4296,7 +4339,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="20" spans="2:54" ht="19.2" customHeight="1">
+    <row r="20" spans="2:54" ht="19.149999999999999" customHeight="1">
       <c r="B20" s="5" t="s">
         <v>40</v>
       </c>
@@ -4379,7 +4422,7 @@
       <c r="AX20" s="1"/>
       <c r="AY20" s="1"/>
     </row>
-    <row r="21" spans="2:54" ht="15.6" thickBot="1">
+    <row r="21" spans="2:54" ht="16.5" thickBot="1">
       <c r="B21" s="20"/>
       <c r="C21" s="21" t="s">
         <v>0</v>
@@ -4493,7 +4536,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="22" spans="2:54" ht="15.6" thickBot="1">
+    <row r="22" spans="2:54" ht="16.5" thickBot="1">
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
       <c r="D22" s="23"/>
@@ -4523,7 +4566,7 @@
       <c r="AB22" s="23"/>
       <c r="AC22" s="23"/>
     </row>
-    <row r="23" spans="2:54" ht="24" thickBot="1">
+    <row r="23" spans="2:54" ht="22.5" thickBot="1">
       <c r="C23" s="3" t="s">
         <v>51</v>
       </c>
@@ -4580,7 +4623,7 @@
       <c r="BA23" s="1"/>
       <c r="BB23" s="1"/>
     </row>
-    <row r="24" spans="2:54" ht="15.6" thickBot="1">
+    <row r="24" spans="2:54" ht="16.5" thickBot="1">
       <c r="B24" s="11" t="s">
         <v>28</v>
       </c>
@@ -4740,7 +4783,9 @@
       <c r="K26" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="L26" s="7"/>
+      <c r="L26" s="8" t="s">
+        <v>718</v>
+      </c>
       <c r="M26" s="8" t="s">
         <v>104</v>
       </c>
@@ -5593,7 +5638,7 @@
       <c r="AB41" s="17"/>
       <c r="AC41" s="19"/>
     </row>
-    <row r="42" spans="2:32" ht="15.6" thickBot="1">
+    <row r="42" spans="2:32" ht="16.5" thickBot="1">
       <c r="B42" s="20"/>
       <c r="C42" s="21" t="s">
         <v>52</v>
@@ -5713,7 +5758,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="2:32" s="1" customFormat="1" ht="14.4" thickBot="1">
+    <row r="45" spans="2:32" s="1" customFormat="1" ht="15" thickBot="1">
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
@@ -5805,7 +5850,7 @@
       </c>
       <c r="AF46" s="4"/>
     </row>
-    <row r="47" spans="2:32" ht="14.4" thickBot="1">
+    <row r="47" spans="2:32" ht="15" thickBot="1">
       <c r="B47" s="24" t="s">
         <v>632</v>
       </c>
@@ -5877,7 +5922,7 @@
       <c r="B48" s="2"/>
       <c r="AF48" s="4"/>
     </row>
-    <row r="49" spans="2:23" s="1" customFormat="1" ht="15.6" thickBot="1">
+    <row r="49" spans="2:23" s="1" customFormat="1" ht="16.5" thickBot="1">
       <c r="B49" s="3" t="s">
         <v>657</v>
       </c>
@@ -5903,7 +5948,7 @@
       <c r="V49" s="2"/>
       <c r="W49" s="2"/>
     </row>
-    <row r="50" spans="2:23" s="35" customFormat="1" ht="13.8">
+    <row r="50" spans="2:23" s="35" customFormat="1" ht="14.25">
       <c r="B50" s="30" t="s">
         <v>658</v>
       </c>
@@ -5963,7 +6008,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="51" spans="2:23" s="32" customFormat="1" ht="14.4" thickBot="1">
+    <row r="51" spans="2:23" s="32" customFormat="1" ht="15" thickBot="1">
       <c r="B51" s="33" t="s">
         <v>659</v>
       </c>
@@ -6023,15 +6068,15 @@
         <v>690</v>
       </c>
     </row>
-    <row r="52" spans="2:23" s="1" customFormat="1" ht="13.8"/>
-    <row r="53" spans="2:23" ht="13.8">
+    <row r="52" spans="2:23" s="1" customFormat="1" ht="14.25"/>
+    <row r="53" spans="2:23" ht="14.25">
       <c r="B53" s="2"/>
     </row>
-    <row r="55" spans="2:23" s="1" customFormat="1" ht="13.8"/>
-    <row r="56" spans="2:23" ht="13.8">
+    <row r="55" spans="2:23" s="1" customFormat="1" ht="14.25"/>
+    <row r="56" spans="2:23" ht="14.25">
       <c r="B56" s="2"/>
     </row>
-    <row r="59" spans="2:23" s="1" customFormat="1" ht="13.8">
+    <row r="59" spans="2:23" s="1" customFormat="1" ht="14.25">
       <c r="B59" s="2"/>
     </row>
   </sheetData>
@@ -6041,24 +6086,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
[sil_euro_latin] Update to keyboard
</commit_message>
<xml_diff>
--- a/release/sil/sil_euro_latin/assets/EuroLatinChart.xlsx
+++ b/release/sil/sil_euro_latin/assets/EuroLatinChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\0WSTech\working\keyboards\release\todo\sil_euro_latin\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SRC\GitHub\keyboards\release\sil\sil_euro_latin\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72DA3E55-19F4-4869-ADF4-3CCB9ED1414B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63543B3-941A-4705-90E3-4FEA0AD683E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="15570" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="720">
   <si>
     <t>a</t>
   </si>
@@ -2179,6 +2179,9 @@
   </si>
   <si>
     <t>J́</t>
+  </si>
+  <si>
+    <t>''</t>
   </si>
 </sst>
 </file>
@@ -2541,7 +2544,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2674,6 +2677,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3015,9 +3021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:BC59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
@@ -3085,7 +3089,7 @@
       <c r="AB3" s="13"/>
       <c r="AC3" s="15"/>
     </row>
-    <row r="4" spans="2:55" ht="21.75">
+    <row r="4" spans="2:55">
       <c r="B4" s="5" t="s">
         <v>27</v>
       </c>
@@ -3432,7 +3436,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="8" spans="2:55" ht="21.75">
+    <row r="8" spans="2:55">
       <c r="B8" s="5" t="s">
         <v>31</v>
       </c>
@@ -3678,7 +3682,7 @@
       <c r="AB10" s="7"/>
       <c r="AC10" s="9"/>
     </row>
-    <row r="11" spans="2:55" ht="21.75">
+    <row r="11" spans="2:55">
       <c r="B11" s="5" t="s">
         <v>33</v>
       </c>
@@ -4106,7 +4110,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="17" spans="2:54" ht="21.75">
+    <row r="17" spans="2:54">
       <c r="B17" s="5" t="s">
         <v>420</v>
       </c>
@@ -4566,7 +4570,7 @@
       <c r="AB22" s="23"/>
       <c r="AC22" s="23"/>
     </row>
-    <row r="23" spans="2:54" ht="22.5" thickBot="1">
+    <row r="23" spans="2:54" ht="16.5" thickBot="1">
       <c r="C23" s="3" t="s">
         <v>51</v>
       </c>
@@ -6016,7 +6020,7 @@
         <v>676</v>
       </c>
       <c r="D51" s="36" t="s">
-        <v>661</v>
+        <v>719</v>
       </c>
       <c r="E51" s="34" t="s">
         <v>677</v>
@@ -6024,7 +6028,7 @@
       <c r="F51" s="34" t="s">
         <v>678</v>
       </c>
-      <c r="G51" s="34" t="s">
+      <c r="G51" s="45" t="s">
         <v>679</v>
       </c>
       <c r="H51" s="34"/>

</xml_diff>

<commit_message>
[sil_euro_latin] Add Wynn to keyboard
</commit_message>
<xml_diff>
--- a/release/sil/sil_euro_latin/assets/EuroLatinChart.xlsx
+++ b/release/sil/sil_euro_latin/assets/EuroLatinChart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20417"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SRC\GitHub\keyboards\release\sil\sil_euro_latin\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F63543B3-941A-4705-90E3-4FEA0AD683E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4815ED15-DA12-4E8D-92EA-B4E4CCB74A88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="105" windowWidth="15570" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="722">
   <si>
     <t>a</t>
   </si>
@@ -2182,6 +2182,12 @@
   </si>
   <si>
     <t>''</t>
+  </si>
+  <si>
+    <t>ƿ</t>
+  </si>
+  <si>
+    <t>Ƿ</t>
   </si>
 </sst>
 </file>
@@ -3021,7 +3027,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:BC59"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y40" sqref="Y40"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75"/>
   <cols>
@@ -4329,7 +4337,9 @@
       </c>
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
-      <c r="Y19" s="7"/>
+      <c r="Y19" s="8" t="s">
+        <v>720</v>
+      </c>
       <c r="Z19" s="8" t="s">
         <v>711</v>
       </c>
@@ -5588,7 +5598,9 @@
       </c>
       <c r="W40" s="7"/>
       <c r="X40" s="7"/>
-      <c r="Y40" s="7"/>
+      <c r="Y40" s="8" t="s">
+        <v>721</v>
+      </c>
       <c r="Z40" s="8" t="s">
         <v>712</v>
       </c>

</xml_diff>